<commit_message>
small style fixes; fixDB script added;
</commit_message>
<xml_diff>
--- a/public/scripts/teachers.xlsx
+++ b/public/scripts/teachers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\TestSystemPack\TestSystem\public\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B68CC7C-5783-4D61-99FD-7264F261FA00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Login</t>
   </si>
@@ -35,11 +34,14 @@
   <si>
     <t>Пароль</t>
   </si>
+  <si>
+    <t>admin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,11 +352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,6 +372,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix FixDb; try to fix checkers
</commit_message>
<xml_diff>
--- a/public/scripts/teachers.xlsx
+++ b/public/scripts/teachers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Login</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ss</t>
   </si>
 </sst>
 </file>
@@ -353,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,6 +389,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>